<commit_message>
Basic genetic algorithm added
</commit_message>
<xml_diff>
--- a/DSO.xlsx
+++ b/DSO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/kwl1y19_soton_ac_uk/Documents/UoS_2023_24/FEEG_DSO/Workbook/DSO-Workbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6678" documentId="8_{42FA694E-ED08-47C7-945B-F9D07721EF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89C9DA02-E7CE-4172-B834-35AB6A132525}"/>
+  <xr:revisionPtr revIDLastSave="8217" documentId="8_{42FA694E-ED08-47C7-945B-F9D07721EF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81E4BE68-F375-4572-9083-5877CC1119AC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{16D0D9C5-2E23-4080-8275-B376E5887C88}"/>
   </bookViews>
@@ -16,35 +16,64 @@
     <sheet name="LineSearch" sheetId="1" r:id="rId1"/>
     <sheet name="Multivariable Optmiser (i)" sheetId="3" r:id="rId2"/>
     <sheet name="Multivariable Optimizer (ii)" sheetId="4" r:id="rId3"/>
-    <sheet name="LineSearchTrueDataPlot" sheetId="2" r:id="rId4"/>
+    <sheet name="Multivariable Optimizer (iii)" sheetId="6" r:id="rId4"/>
+    <sheet name="LineSearchTrueDataPlot" sheetId="2" r:id="rId5"/>
+    <sheet name="Misc" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Multivariable Optimizer (ii)'!$B$3:$C$3</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Multivariable Optmiser (i)'!$P$56</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Multivariable Optimizer (ii)'!$D$3</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'Multivariable Optmiser (i)'!$S$56</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000000000001</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -90,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="118">
   <si>
     <t>f(x) = Ax^4 +Bx^3 + C</t>
   </si>
@@ -362,12 +391,152 @@
   <si>
     <t>Conjugate have different lambdas for each iteration!</t>
   </si>
+  <si>
+    <t>Problem: f(x) = x1-x2+2*x1x2^2+x2^3</t>
+  </si>
+  <si>
+    <t>Solver Solution</t>
+  </si>
+  <si>
+    <t>f(x) Minima</t>
+  </si>
+  <si>
+    <t>Hooke &amp; Jeeves</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>decision</t>
+  </si>
+  <si>
+    <t>Step Length</t>
+  </si>
+  <si>
+    <t>Base Point</t>
+  </si>
+  <si>
+    <t>explore x1</t>
+  </si>
+  <si>
+    <t>explore x2</t>
+  </si>
+  <si>
+    <t>New Base Point</t>
+  </si>
+  <si>
+    <t>Pattern Move</t>
+  </si>
+  <si>
+    <t>Note pattern move is based on vetor from last base point to new base point</t>
+  </si>
+  <si>
+    <t>Design a representation
+Decide how to initialise a population
+Design a way of mapping a genotype to a phenotype
+Design a way of evaluating an individual
+Design suitable mutation operators
+Design suitable recombination operators
+Decide how to manage population
+Decide how to select individuals to be parents
+Decide how to select individuals to be replaced
+Decide when to stop the algorithm
+Scale integers to get float
+Mutation is important and should be controllable
+Ranked based parents selection is used, where the "grades" always have the same proportions
+Recombination : Exploitation operator
+Mutation : Exploration operator
+Stopping criterion
+Never draw any conclusion from a single run
+Exploration vs Explotation:
+1. Too much exploration = sample unknown regions: random search no convergence
+2. Too much exploitation = Try to improve the best-so-far individuals:  local search only, convergence to a local optimum</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>UB</t>
+  </si>
+  <si>
+    <t>Random no. 1</t>
+  </si>
+  <si>
+    <t>Random no. 2</t>
+  </si>
+  <si>
+    <t>Random no. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genetic Algorithm:
+6 BIT BINARY, SINGLE VARIABLE, POPULATION OF DESIGNS </t>
+  </si>
+  <si>
+    <t>GA Parameters</t>
+  </si>
+  <si>
+    <t>Bits</t>
+  </si>
+  <si>
+    <t>Min/max ADC</t>
+  </si>
+  <si>
+    <t>Parent Bit String (la DNA)</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Bit Dec Val</t>
+  </si>
+  <si>
+    <t>Converts ADC to proper Bin</t>
+  </si>
+  <si>
+    <t>idk how to describe</t>
+  </si>
+  <si>
+    <t>lol</t>
+  </si>
+  <si>
+    <t>P1 ADC</t>
+  </si>
+  <si>
+    <t>P2 ADC</t>
+  </si>
+  <si>
+    <t>Float to 'Bit'</t>
+  </si>
+  <si>
+    <t>Cross Over Point</t>
+  </si>
+  <si>
+    <t>i.e. Bit to start splicing DNA</t>
+  </si>
+  <si>
+    <t>Children Bit String</t>
+  </si>
+  <si>
+    <t>Total Bit</t>
+  </si>
+  <si>
+    <t>Mutation point</t>
+  </si>
+  <si>
+    <t>Scaled Results</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,8 +575,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,6 +628,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -686,27 +891,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -722,12 +909,54 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2803,6 +3032,346 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Hookes and Jeeves</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Multivariable Optimizer (ii)'!$C$5,'Multivariable Optimizer (ii)'!$C$10,'Multivariable Optimizer (ii)'!$C$11,'Multivariable Optimizer (ii)'!$C$16,'Multivariable Optimizer (ii)'!$C$17,'Multivariable Optimizer (ii)'!$C$21,'Multivariable Optimizer (ii)'!$C$22)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.50000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.70000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.1000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Multivariable Optimizer (ii)'!$D$5,'Multivariable Optimizer (ii)'!$D$10,'Multivariable Optimizer (ii)'!$D$11,'Multivariable Optimizer (ii)'!$D$16,'Multivariable Optimizer (ii)'!$D$17,'Multivariable Optimizer (ii)'!$D$21,'Multivariable Optimizer (ii)'!$D$22,'Multivariable Optimizer (ii)'!$D$26,'Multivariable Optimizer (ii)'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F01F-4DC9-A666-01B15182A95F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="934317168"/>
+        <c:axId val="838394880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="934317168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="838394880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="838394880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="934317168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2844,6 +3413,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3915,6 +4524,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3992,6 +5117,225 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{293376E3-6462-52F7-4975-80A7689EB2A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>971549</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBA5E0FC-C2E7-D5D9-A697-6DA401886973}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="39580" t="48845" r="36485" b="10431"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6534149" y="13182600"/>
+          <a:ext cx="1704975" cy="2152650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4926EE2E-C9DD-48D9-9685-5E2C399DE559}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="71805" t="14788" r="4260" b="44488"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6619875" y="15868650"/>
+          <a:ext cx="1704975" cy="2152650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB3AD432-8062-48DD-B84B-745589437B56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect t="913" r="381" b="-20"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9829800" y="12725400"/>
+          <a:ext cx="7096125" cy="5238750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>551467</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58B26258-620C-EAD2-360A-275ED1EBDF25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7866667" cy="5685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4330,10 +5674,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="34"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -4351,8 +5695,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
       <c r="C5">
         <v>0</v>
       </c>
@@ -4368,8 +5712,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
       <c r="C6">
         <v>0.2</v>
       </c>
@@ -4385,8 +5729,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
       <c r="C7">
         <v>0.4</v>
       </c>
@@ -4402,8 +5746,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
       <c r="C8">
         <v>0.6</v>
       </c>
@@ -4413,8 +5757,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
       <c r="C9">
         <v>0.8</v>
       </c>
@@ -4430,8 +5774,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -4441,8 +5785,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
       <c r="C11">
         <v>1.2</v>
       </c>
@@ -4452,8 +5796,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
       <c r="C12">
         <v>1.4</v>
       </c>
@@ -4463,8 +5807,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
       <c r="C13">
         <v>1.6</v>
       </c>
@@ -4474,8 +5818,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
       <c r="C14">
         <v>1.8</v>
       </c>
@@ -4485,8 +5829,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
       <c r="C15">
         <v>2</v>
       </c>
@@ -4922,10 +6266,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S23" s="22" t="s">
+      <c r="S23" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="T23" s="22"/>
+      <c r="T23" s="36"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24">
@@ -5339,7 +6683,7 @@
       </c>
     </row>
     <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B31">
@@ -5392,7 +6736,7 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="35"/>
       <c r="B32">
         <v>2</v>
       </c>
@@ -5444,7 +6788,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+      <c r="A33" s="35"/>
       <c r="B33">
         <v>3</v>
       </c>
@@ -5496,7 +6840,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
+      <c r="A34" s="35"/>
       <c r="B34">
         <v>4</v>
       </c>
@@ -5516,7 +6860,7 @@
         <v>2.3143423435168815</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G33:G40" si="26">E33</f>
+        <f t="shared" ref="G34:G40" si="26">E33</f>
         <v>1.5373371924746755</v>
       </c>
       <c r="H34">
@@ -5545,7 +6889,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="35"/>
       <c r="B35">
         <v>5</v>
       </c>
@@ -5594,7 +6938,7 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="35"/>
       <c r="B36">
         <v>6</v>
       </c>
@@ -5643,7 +6987,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+      <c r="A37" s="35"/>
       <c r="B37">
         <v>7</v>
       </c>
@@ -5692,7 +7036,7 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
+      <c r="A38" s="35"/>
       <c r="B38">
         <v>8</v>
       </c>
@@ -5741,7 +7085,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
+      <c r="A39" s="35"/>
       <c r="B39">
         <v>9</v>
       </c>
@@ -5790,7 +7134,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
+      <c r="A40" s="35"/>
       <c r="B40">
         <v>10</v>
       </c>
@@ -5889,7 +7233,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="32" t="s">
         <v>40</v>
       </c>
       <c r="B43">
@@ -5939,7 +7283,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
+      <c r="A44" s="35"/>
       <c r="B44">
         <v>2</v>
       </c>
@@ -5989,7 +7333,7 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
+      <c r="A45" s="35"/>
       <c r="B45">
         <v>3</v>
       </c>
@@ -6002,7 +7346,7 @@
         <v>2.315130674643628</v>
       </c>
       <c r="E45" s="11">
-        <f t="shared" ref="E44:E52" si="33">C45+($T$20)*(G45-C45)</f>
+        <f t="shared" ref="E45:E52" si="33">C45+($T$20)*(G45-C45)</f>
         <v>1.4700626974056508</v>
       </c>
       <c r="F45">
@@ -6018,7 +7362,7 @@
         <v>2.3679575387602441</v>
       </c>
       <c r="I45" s="5">
-        <f t="shared" ref="I44:I52" si="37">((H45-F45)*(E45^2-C45^2)+(D45-F45)*(G45^2-E45^2))/(2*((H45-F45)*(E45-C45)+(D45-F45)*(G45-E45)))</f>
+        <f t="shared" ref="I45:I52" si="37">((H45-F45)*(E45^2-C45^2)+(D45-F45)*(G45^2-E45^2))/(2*((H45-F45)*(E45-C45)+(D45-F45)*(G45-E45)))</f>
         <v>1.4999837323892411</v>
       </c>
       <c r="J45" s="5">
@@ -6039,7 +7383,7 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="35"/>
       <c r="B46">
         <v>4</v>
       </c>
@@ -6089,7 +7433,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
+      <c r="A47" s="35"/>
       <c r="B47">
         <v>5</v>
       </c>
@@ -6139,7 +7483,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
+      <c r="A48" s="35"/>
       <c r="B48">
         <v>6</v>
       </c>
@@ -6189,7 +7533,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
+      <c r="A49" s="35"/>
       <c r="B49">
         <v>7</v>
       </c>
@@ -6239,7 +7583,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
+      <c r="A50" s="35"/>
       <c r="B50">
         <v>8</v>
       </c>
@@ -6289,7 +7633,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
+      <c r="A51" s="35"/>
       <c r="B51">
         <v>9</v>
       </c>
@@ -6339,7 +7683,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
+      <c r="A52" s="35"/>
       <c r="B52">
         <v>10</v>
       </c>
@@ -6416,7 +7760,7 @@
       <c r="K54" s="17"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B55">
@@ -6445,7 +7789,7 @@
       <c r="K55" s="17"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
+      <c r="A56" s="33"/>
       <c r="B56">
         <v>2</v>
       </c>
@@ -6477,7 +7821,7 @@
       <c r="K56" s="17"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
+      <c r="A57" s="33"/>
       <c r="B57">
         <v>3</v>
       </c>
@@ -6507,7 +7851,7 @@
       <c r="K57" s="17"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
+      <c r="A58" s="33"/>
       <c r="B58">
         <v>4</v>
       </c>
@@ -6537,7 +7881,7 @@
       <c r="K58" s="17"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
+      <c r="A59" s="33"/>
       <c r="B59">
         <v>5</v>
       </c>
@@ -6567,7 +7911,7 @@
       <c r="K59" s="17"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
+      <c r="A60" s="33"/>
       <c r="B60">
         <v>6</v>
       </c>
@@ -6593,7 +7937,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="33"/>
       <c r="B61">
         <v>7</v>
       </c>
@@ -6619,7 +7963,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
+      <c r="A62" s="33"/>
       <c r="B62">
         <v>8</v>
       </c>
@@ -6645,7 +7989,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
+      <c r="A63" s="33"/>
       <c r="B63">
         <v>9</v>
       </c>
@@ -6671,7 +8015,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="19"/>
+      <c r="A64" s="33"/>
       <c r="B64">
         <v>10</v>
       </c>
@@ -6697,7 +8041,7 @@
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="19"/>
+      <c r="A65" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6720,8 +8064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC08575-9C70-4C28-95BC-F2FE05F8FA47}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6737,7 +8081,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="24" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="8"/>
@@ -6745,66 +8089,66 @@
       <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="26">
         <v>1</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="28">
         <v>-2</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="28">
         <v>2</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="28">
         <v>1</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="30">
         <v>2</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="22">
         <v>-1.9999996374097115</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="22">
         <v>1.4999992725118474</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="23">
         <f>$B$2*B7+$B$3*C7+$B$4*B7*C7+$B$5*B7^2+$B$6*C7^2</f>
         <v>-2.4999999999993392</v>
       </c>
@@ -6812,17 +8156,17 @@
       <c r="U7" s="17"/>
     </row>
     <row r="8" spans="1:21" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39" t="s">
+      <c r="C8" s="37"/>
+      <c r="D8" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="38"/>
       <c r="T8" s="17"/>
       <c r="U8" s="17"/>
     </row>
@@ -6886,7 +8230,7 @@
       <c r="U9" s="17"/>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="39" t="s">
         <v>76</v>
       </c>
       <c r="C10">
@@ -6938,7 +8282,7 @@
       <c r="U10" s="17"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="40"/>
       <c r="C11">
         <v>0.5</v>
       </c>
@@ -6988,7 +8332,7 @@
       <c r="U11" s="17"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="40"/>
       <c r="C12" s="15">
         <v>0.5</v>
       </c>
@@ -7038,7 +8382,7 @@
       <c r="U12" s="17"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="40"/>
       <c r="C13" s="15">
         <v>0.5</v>
       </c>
@@ -7088,7 +8432,7 @@
       <c r="U13" s="17"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="40"/>
       <c r="C14" s="15">
         <v>0.5</v>
       </c>
@@ -7138,7 +8482,7 @@
       <c r="U14" s="17"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="40"/>
       <c r="C15" s="15">
         <v>0.5</v>
       </c>
@@ -7191,7 +8535,7 @@
       <c r="U15" s="17"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="40"/>
       <c r="C16" s="15">
         <v>0.5</v>
       </c>
@@ -7244,7 +8588,7 @@
       <c r="U16" s="17"/>
     </row>
     <row r="17" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="4" t="s">
         <v>73</v>
       </c>
@@ -7301,7 +8645,7 @@
       <c r="U17" s="17"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="19"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -7338,7 +8682,7 @@
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
-      <c r="P18" s="26">
+      <c r="P18" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q18" s="15">
@@ -7359,7 +8703,7 @@
       <c r="U18" s="17"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="19"/>
       <c r="B19">
         <v>2</v>
       </c>
@@ -7398,7 +8742,7 @@
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
-      <c r="P19" s="26">
+      <c r="P19" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q19" s="15">
@@ -7417,7 +8761,7 @@
       <c r="U19" s="17"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="19"/>
       <c r="B20">
         <v>3</v>
       </c>
@@ -7456,7 +8800,7 @@
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
-      <c r="P20" s="26">
+      <c r="P20" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q20" s="15">
@@ -7475,7 +8819,7 @@
       <c r="U20" s="17"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="15">
         <v>4</v>
       </c>
@@ -7511,7 +8855,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="P21" s="26">
+      <c r="P21" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q21" s="15">
@@ -7530,7 +8874,7 @@
       <c r="U21" s="17"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="15">
         <v>5</v>
       </c>
@@ -7566,7 +8910,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="P22" s="26">
+      <c r="P22" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q22" s="15">
@@ -7620,7 +8964,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="P23" s="26">
+      <c r="P23" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q23" s="15">
@@ -7674,7 +9018,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="P24" s="26">
+      <c r="P24" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q24" s="15">
@@ -7728,7 +9072,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="P25" s="26">
+      <c r="P25" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q25" s="15">
@@ -7782,7 +9126,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="P26" s="26">
+      <c r="P26" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q26" s="15">
@@ -7836,7 +9180,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="P27" s="26">
+      <c r="P27" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q27" s="15">
@@ -7893,7 +9237,7 @@
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
-      <c r="P28" s="26">
+      <c r="P28" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q28" s="15">
@@ -7950,7 +9294,7 @@
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
-      <c r="P29" s="26">
+      <c r="P29" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q29" s="15">
@@ -8007,7 +9351,7 @@
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
-      <c r="P30" s="26">
+      <c r="P30" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q30" s="15">
@@ -8064,7 +9408,7 @@
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
-      <c r="P31" s="26">
+      <c r="P31" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q31" s="15">
@@ -8119,7 +9463,7 @@
       <c r="M32" s="15"/>
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
-      <c r="P32" s="26">
+      <c r="P32" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q32" s="15">
@@ -8174,7 +9518,7 @@
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
-      <c r="P33" s="26">
+      <c r="P33" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q33" s="15">
@@ -8229,7 +9573,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
-      <c r="P34" s="26">
+      <c r="P34" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q34" s="15">
@@ -8284,7 +9628,7 @@
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
-      <c r="P35" s="26">
+      <c r="P35" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q35" s="15">
@@ -8339,7 +9683,7 @@
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
-      <c r="P36" s="26">
+      <c r="P36" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q36" s="15">
@@ -8394,7 +9738,7 @@
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
-      <c r="P37" s="26">
+      <c r="P37" s="20">
         <v>0.38461538461538486</v>
       </c>
       <c r="Q37" s="15">
@@ -8510,7 +9854,7 @@
         <v>-1</v>
       </c>
       <c r="O40" s="15"/>
-      <c r="P40" s="26">
+      <c r="P40" s="20">
         <v>0.29411764705882354</v>
       </c>
       <c r="Q40" s="15">
@@ -8570,7 +9914,7 @@
         <f>-G41+(ABS(H41)^2)/(ABS(H40)^2)*N40</f>
         <v>1.765879239951629</v>
       </c>
-      <c r="P41" s="26">
+      <c r="P41" s="20">
         <v>0.60331111194513309</v>
       </c>
       <c r="Q41" s="15">
@@ -8634,7 +9978,7 @@
         <v>-0.18393708570421696</v>
       </c>
       <c r="O42" s="15"/>
-      <c r="P42" s="26">
+      <c r="P42" s="20">
         <v>0.32342972772715034</v>
       </c>
       <c r="Q42" s="15">
@@ -8695,7 +10039,7 @@
         <v>0.52213760929620967</v>
       </c>
       <c r="O43" s="15"/>
-      <c r="P43" s="26">
+      <c r="P43" s="20">
         <v>0.29197016223648109</v>
       </c>
       <c r="Q43" s="15">
@@ -8756,7 +10100,7 @@
         <v>2.5919373659344283E-2</v>
       </c>
       <c r="O44" s="15"/>
-      <c r="P44" s="26">
+      <c r="P44" s="20">
         <v>0.56249796897019011</v>
       </c>
       <c r="Q44" s="15">
@@ -8816,7 +10160,7 @@
         <v>0.25115147097090479</v>
       </c>
       <c r="O45" s="15"/>
-      <c r="P45" s="26">
+      <c r="P45" s="20">
         <v>0.36612748673208401</v>
       </c>
       <c r="Q45" s="15">
@@ -8877,7 +10221,7 @@
         <v>-3.3298262604043519E-2</v>
       </c>
       <c r="O46" s="15"/>
-      <c r="P46" s="26">
+      <c r="P46" s="20">
         <v>0.30005911902049365</v>
       </c>
       <c r="Q46" s="15">
@@ -8938,7 +10282,7 @@
         <v>5.6940938915434738E-2</v>
       </c>
       <c r="O47" s="15"/>
-      <c r="P47" s="26">
+      <c r="P47" s="20">
         <v>0.48933482506928988</v>
       </c>
       <c r="Q47" s="15">
@@ -8999,7 +10343,7 @@
         <v>2.439498680734585E-3</v>
       </c>
       <c r="O48" s="15"/>
-      <c r="P48" s="26">
+      <c r="P48" s="20">
         <v>0.4148955098698987</v>
       </c>
       <c r="Q48" s="15">
@@ -9060,7 +10404,7 @@
         <v>2.1708480546861045E-2</v>
       </c>
       <c r="O49" s="15"/>
-      <c r="P49" s="26">
+      <c r="P49" s="20">
         <v>0.25973886907559873</v>
       </c>
       <c r="Q49" s="15">
@@ -9121,7 +10465,7 @@
         <v>5.1811770542272697E-4</v>
       </c>
       <c r="O50" s="15"/>
-      <c r="P50" s="26">
+      <c r="P50" s="20">
         <v>0.55130966089701117</v>
       </c>
       <c r="Q50" s="15">
@@ -9182,7 +10526,7 @@
         <v>9.7968123603703276E-3</v>
       </c>
       <c r="O51" s="15"/>
-      <c r="P51" s="26">
+      <c r="P51" s="20">
         <v>0.43640512432106915</v>
       </c>
       <c r="Q51" s="15">
@@ -9243,7 +10587,7 @@
         <v>-1.1190266711390551E-3</v>
       </c>
       <c r="O52" s="15"/>
-      <c r="P52" s="26">
+      <c r="P52" s="20">
         <v>0.21508356181710694</v>
       </c>
       <c r="Q52" s="15">
@@ -9304,7 +10648,7 @@
         <v>4.5567854208624042E-4</v>
       </c>
       <c r="O53" s="15"/>
-      <c r="P53" s="26">
+      <c r="P53" s="20">
         <v>0.79278881141926583</v>
       </c>
       <c r="Q53" s="15">
@@ -9365,7 +10709,7 @@
         <v>2.2994596581635447E-4</v>
       </c>
       <c r="O54" s="15"/>
-      <c r="P54" s="26">
+      <c r="P54" s="20">
         <v>0.31201479130228971</v>
       </c>
       <c r="Q54" s="15">
@@ -9426,7 +10770,7 @@
         <v>-6.1318342278445954E-5</v>
       </c>
       <c r="O55" s="15"/>
-      <c r="P55" s="26">
+      <c r="P55" s="20">
         <v>0.20931134670729132</v>
       </c>
       <c r="Q55" s="15">
@@ -9487,7 +10831,7 @@
         <v>-4.4524895575110093E-6</v>
       </c>
       <c r="O56" s="15"/>
-      <c r="P56" s="26">
+      <c r="P56" s="20">
         <v>0</v>
       </c>
       <c r="Q56" s="15">
@@ -9548,7 +10892,7 @@
         <v>-8.498884268365893E-6</v>
       </c>
       <c r="O57" s="15"/>
-      <c r="P57" s="26">
+      <c r="P57" s="20">
         <v>0</v>
       </c>
       <c r="Q57" s="15">
@@ -9609,7 +10953,7 @@
         <v>-1.2545278979220777E-5</v>
       </c>
       <c r="O58" s="15"/>
-      <c r="P58" s="26">
+      <c r="P58" s="20">
         <v>0</v>
       </c>
       <c r="Q58" s="15">
@@ -9670,7 +11014,7 @@
         <v>-1.659167369007566E-5</v>
       </c>
       <c r="O59" s="15"/>
-      <c r="P59" s="26">
+      <c r="P59" s="20">
         <v>0</v>
       </c>
       <c r="Q59" s="15">
@@ -9700,11 +11044,1288 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05066E6-B41F-499D-9F3E-6508D758A95E}">
+  <dimension ref="A1:K73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="18" customWidth="1"/>
+    <col min="10" max="10" width="83.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7">
+        <v>-53687091.200000003</v>
+      </c>
+      <c r="C3" s="7">
+        <v>-35791499.799999997</v>
+      </c>
+      <c r="D3" s="7">
+        <f>B3-C3+(2*B3*(C3^2))+C3^3</f>
+        <v>-1.8339974259469579E+23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="44"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <f>C5-D5+2*C5*D5^2+D5^3</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6">
+        <f>$C$5+$H$5</f>
+        <v>0.1</v>
+      </c>
+      <c r="D6">
+        <f>$D$5</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" ref="E6:E26" si="0">C6-D6+2*C6*D6^2+D6^3</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F6">
+        <f>E6-E5</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G6" t="str">
+        <f>IF(F6&gt;0,"Reject", "Accept")</f>
+        <v>Reject</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="18">
+        <f>$C$5-$H$5</f>
+        <v>-0.1</v>
+      </c>
+      <c r="D7" s="18">
+        <f>$D$5</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="F7" s="18">
+        <f t="shared" ref="F7:F26" si="1">E7-E6</f>
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="G7" s="18" t="str">
+        <f t="shared" ref="G7:G27" si="2">IF(F7&gt;0,"Reject", "Accept")</f>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="18">
+        <f>$C$5-$H$5</f>
+        <v>-0.1</v>
+      </c>
+      <c r="D8" s="18">
+        <f>$D$5+$H$5</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.11099999999999977</v>
+      </c>
+      <c r="F8" s="18">
+        <f t="shared" si="1"/>
+        <v>0.18900000000000028</v>
+      </c>
+      <c r="G8" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Reject</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="18">
+        <f>$C$5-$H$5</f>
+        <v>-0.1</v>
+      </c>
+      <c r="D9" s="18">
+        <f>$D$5-$H$5</f>
+        <v>0.9</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.43299999999999983</v>
+      </c>
+      <c r="F9" s="18">
+        <f t="shared" si="1"/>
+        <v>-0.32200000000000006</v>
+      </c>
+      <c r="G9" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10">
+        <f>C9</f>
+        <v>-0.1</v>
+      </c>
+      <c r="D10">
+        <f>D9</f>
+        <v>0.9</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.43299999999999983</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="18">
+        <f>$C$10-(C5-C10)</f>
+        <v>-0.2</v>
+      </c>
+      <c r="D11" s="18">
+        <f>$D$10-(D5-D10)</f>
+        <v>0.8</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" ref="E11" si="3">C11-D11+2*C11*D11^2+D11^3</f>
+        <v>-0.74399999999999988</v>
+      </c>
+      <c r="F11" s="18">
+        <f>E11-E9</f>
+        <v>-0.31100000000000005</v>
+      </c>
+      <c r="G11" s="18" t="str">
+        <f>IF(F11&gt;0,"Reject", "Accept")</f>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12">
+        <f>$C$11+$H$5</f>
+        <v>-0.1</v>
+      </c>
+      <c r="D12">
+        <f>$D$11</f>
+        <v>0.8</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.5159999999999999</v>
+      </c>
+      <c r="F12" s="18">
+        <f>E12-E11</f>
+        <v>0.22799999999999998</v>
+      </c>
+      <c r="G12" s="18" t="str">
+        <f>IF(F12&gt;0,"Reject", "Accept")</f>
+        <v>Reject</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="18">
+        <f>$C$11-$H$5</f>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="D13" s="18">
+        <f>$D$11</f>
+        <v>0.8</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.97200000000000009</v>
+      </c>
+      <c r="F13" s="18">
+        <f>E13-E12</f>
+        <v>-0.45600000000000018</v>
+      </c>
+      <c r="G13" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14">
+        <f>C13</f>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="D14">
+        <f>$D$11+$H$5</f>
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.95700000000000029</v>
+      </c>
+      <c r="F14" s="18">
+        <f>E14-E13</f>
+        <v>1.4999999999999791E-2</v>
+      </c>
+      <c r="G14" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Reject</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="18">
+        <f>C14</f>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="D15" s="18">
+        <f>$D$11-$H$5</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.95099999999999996</v>
+      </c>
+      <c r="F15" s="18">
+        <f>E15-E14</f>
+        <v>6.0000000000003384E-3</v>
+      </c>
+      <c r="G15" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Reject</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16">
+        <f>C15</f>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="D16">
+        <f>D13</f>
+        <v>0.8</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.97200000000000009</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="18">
+        <f>C16-(C10-C16)</f>
+        <v>-0.50000000000000011</v>
+      </c>
+      <c r="D17" s="18">
+        <f>D16-(D10-D16)</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.3470000000000004</v>
+      </c>
+      <c r="F17" s="18">
+        <f>E17-E16</f>
+        <v>-0.37500000000000033</v>
+      </c>
+      <c r="G17" s="18" t="str">
+        <f>IF(F17&gt;0,"Reject", "Accept")</f>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18">
+        <f>C17-H5</f>
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="D18">
+        <f>D17</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.5450000000000004</v>
+      </c>
+      <c r="F18" s="18">
+        <f>E18-E17</f>
+        <v>-0.19799999999999995</v>
+      </c>
+      <c r="G18" s="18" t="str">
+        <f>IF(F18&gt;0,"Reject", "Accept")</f>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19">
+        <f>C18</f>
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="D19">
+        <f>D17-H5</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.4160000000000004</v>
+      </c>
+      <c r="F19" s="18">
+        <f>E19-E18</f>
+        <v>0.129</v>
+      </c>
+      <c r="G19" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Reject</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="18">
+        <f t="shared" ref="C20:C26" si="4">C19-$H$5</f>
+        <v>-0.70000000000000007</v>
+      </c>
+      <c r="D20" s="18">
+        <f>D17+H5</f>
+        <v>0.8</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.8840000000000003</v>
+      </c>
+      <c r="F20" s="18">
+        <f t="shared" si="1"/>
+        <v>-0.46799999999999997</v>
+      </c>
+      <c r="G20" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="18">
+        <f>C20</f>
+        <v>-0.70000000000000007</v>
+      </c>
+      <c r="D21" s="18">
+        <f>D20</f>
+        <v>0.8</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.8840000000000003</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="18">
+        <f>C21-(C16-C21)</f>
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="D22" s="18">
+        <f>D21-(D16-D21)</f>
+        <v>0.8</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="0"/>
+        <v>-2.7960000000000007</v>
+      </c>
+      <c r="F22" s="18">
+        <f>E22-E21</f>
+        <v>-0.91200000000000037</v>
+      </c>
+      <c r="G22" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="18">
+        <f>C22-H5</f>
+        <v>-1.2000000000000002</v>
+      </c>
+      <c r="D23" s="18">
+        <f>D22</f>
+        <v>0.8</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="0"/>
+        <v>-3.0240000000000005</v>
+      </c>
+      <c r="F23" s="18">
+        <f t="shared" ref="F23:F27" si="5">E23-E22</f>
+        <v>-0.22799999999999976</v>
+      </c>
+      <c r="G23" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="18">
+        <f>C23</f>
+        <v>-1.2000000000000002</v>
+      </c>
+      <c r="D24" s="18">
+        <f>D23-H5</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="0"/>
+        <v>-2.7330000000000005</v>
+      </c>
+      <c r="F24" s="18">
+        <f t="shared" si="5"/>
+        <v>0.29099999999999993</v>
+      </c>
+      <c r="G24" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Reject</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="18">
+        <f>C24</f>
+        <v>-1.2000000000000002</v>
+      </c>
+      <c r="D25" s="18">
+        <f>D22+H5</f>
+        <v>0.9</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="0"/>
+        <v>-3.3150000000000004</v>
+      </c>
+      <c r="F25" s="18">
+        <f t="shared" si="5"/>
+        <v>-0.58199999999999985</v>
+      </c>
+      <c r="G25" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="18">
+        <f>C25</f>
+        <v>-1.2000000000000002</v>
+      </c>
+      <c r="D26" s="18">
+        <f>D25</f>
+        <v>0.9</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="0"/>
+        <v>-3.3150000000000004</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="18">
+        <f>C26-(C21-C26)</f>
+        <v>-1.7000000000000002</v>
+      </c>
+      <c r="D27" s="18">
+        <f>D26-(D21-D26)</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" ref="E27" si="6">C27-D27+2*C27*D27^2+D27^3</f>
+        <v>-5.1000000000000005</v>
+      </c>
+      <c r="F27" s="18">
+        <f t="shared" si="5"/>
+        <v>-1.7850000000000001</v>
+      </c>
+      <c r="G27" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Accept</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="44"/>
+    </row>
+    <row r="30" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="J31" s="43"/>
+    </row>
+    <row r="32" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="18">
+        <v>6</v>
+      </c>
+      <c r="J32" s="43"/>
+    </row>
+    <row r="33" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="18">
+        <v>0</v>
+      </c>
+      <c r="C33" s="18">
+        <f>(2^B32)-1</f>
+        <v>63</v>
+      </c>
+      <c r="J33" s="43"/>
+    </row>
+    <row r="34" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I34" s="44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8">
+        <v>-1</v>
+      </c>
+      <c r="D35" s="55">
+        <v>-0.42857000000000001</v>
+      </c>
+      <c r="E35" s="55">
+        <v>4.7620000000000003E-2</v>
+      </c>
+      <c r="F35" s="8">
+        <v>1</v>
+      </c>
+      <c r="G35" s="8">
+        <f ca="1">RAND()</f>
+        <v>0.96456720362692883</v>
+      </c>
+      <c r="H35" s="8">
+        <f t="shared" ref="H35:I35" ca="1" si="7">RAND()</f>
+        <v>0.40430807618073339</v>
+      </c>
+      <c r="I35" s="8">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.29281474835444654</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36">
+        <f>(ABS(D35-$C$35)/($F$35-$C$35))*($C$33-$B$33)</f>
+        <v>18.000045</v>
+      </c>
+      <c r="E36" s="18">
+        <f>(ABS(E35-$C$35)/($F$35-$C$35))*($C$33-$B$33)</f>
+        <v>33.000030000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="50">
+        <v>5</v>
+      </c>
+      <c r="D38" s="49">
+        <f>FLOOR(D36/2^C38,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="49">
+        <f>FLOOR(E36/2^C38,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F38" s="50">
+        <f>2^C38</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="50">
+        <v>4</v>
+      </c>
+      <c r="D39" s="49">
+        <f>FLOOR((D36-D38*2^C38)/(2^C39),1)</f>
+        <v>1</v>
+      </c>
+      <c r="E39" s="49">
+        <f>FLOOR((E36-E38*2^C38)/(2^C39),1)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="50">
+        <f t="shared" ref="F39:F43" si="8">2^C39</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="50">
+        <v>3</v>
+      </c>
+      <c r="D40" s="49">
+        <f>FLOOR((D36-D38*2^C38-D39*2^C39)/(2^C40),1)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="49">
+        <f>FLOOR((E36-E38*2^C38-E39*2^C39)/(2^C40),1)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="50">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="50">
+        <v>2</v>
+      </c>
+      <c r="D41" s="49">
+        <f>FLOOR((D36-D38*2^C38-D39*2^C39-D40*2^C40)/(2^C41),1)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="49">
+        <f>FLOOR((E36-E38*2^C38-E39*2^C39-E40*2^C40)/(2^C41),1)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="50">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="50">
+        <v>1</v>
+      </c>
+      <c r="D42" s="49">
+        <f>FLOOR((D36-D38*2^C38-D39*2^C39-D40*2^C40-D41*2^C41)/(2^C42),1)</f>
+        <v>1</v>
+      </c>
+      <c r="E42" s="49">
+        <f>FLOOR((E36-E38*2^C38-E39*2^C39-E40*2^C40-E41*2^C41)/(2^C42),1)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="50">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="50">
+        <v>0</v>
+      </c>
+      <c r="D43" s="49">
+        <f>FLOOR((D36-D38*2^C38-D39*2^C39-D40*2^C40-D41*2^C41-D42*2^C42)/(2^C43),1)</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="49">
+        <f>FLOOR((E36-E38*2^C38-E39*2^C39-E40*2^C40-E41*2^C41-E42*2^C42)/(2^C43),1)</f>
+        <v>1</v>
+      </c>
+      <c r="F43" s="50">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="F44" s="50"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="53">
+        <f>D38*2^C38+D39*2^C39+D40*2^C40+D41*2^C41+D42*2^C42+D43*2^C43</f>
+        <v>18</v>
+      </c>
+      <c r="E45" s="53">
+        <f>E38*2^C38+E39*2^C39+E40*2^C40+E41*2^C41+E42*2^C42+E43*2^C43</f>
+        <v>33</v>
+      </c>
+      <c r="F45" s="50"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="54">
+        <f ca="1">FLOOR($B$32*G35,1)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="G50" s="18"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="20">
+        <v>5</v>
+      </c>
+      <c r="D51" s="46">
+        <f ca="1">IF(G47&gt;=1,E38,D38)</f>
+        <v>1</v>
+      </c>
+      <c r="E51" s="46">
+        <f ca="1">IF(G47&gt;=1,D38,E38)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="20">
+        <f>2^C51</f>
+        <v>32</v>
+      </c>
+      <c r="G51" s="18"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="20">
+        <v>4</v>
+      </c>
+      <c r="D52" s="46">
+        <f ca="1">IF(G47&gt;=2,E39,D39)</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="46">
+        <f ca="1">IF(G47&gt;=2,D39,E39)</f>
+        <v>1</v>
+      </c>
+      <c r="F52" s="20">
+        <f t="shared" ref="F52:F56" si="9">2^C52</f>
+        <v>16</v>
+      </c>
+      <c r="G52" s="18"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="20">
+        <v>3</v>
+      </c>
+      <c r="D53" s="46">
+        <f ca="1">IF(G47&gt;=3,E40,D40)</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="46">
+        <f ca="1">IF(G47&gt;=3,D40,E40)</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="20">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G53" s="18"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="20">
+        <v>2</v>
+      </c>
+      <c r="D54" s="46">
+        <f ca="1">IF(G47&gt;=4,E41,D41)</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="46">
+        <f ca="1">IF(G47&gt;=4,D41,E41)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="20">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G54" s="18"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="20">
+        <v>1</v>
+      </c>
+      <c r="D55" s="46">
+        <f ca="1">IF(G47&gt;=5,E42,D42)</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="46">
+        <f ca="1">IF(G47&gt;=5,D42,E42)</f>
+        <v>1</v>
+      </c>
+      <c r="F55" s="20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="G55" s="18"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="20">
+        <v>0</v>
+      </c>
+      <c r="D56" s="46">
+        <f ca="1">IF(G47&gt;=6,E43,D43)</f>
+        <v>0</v>
+      </c>
+      <c r="E56" s="46">
+        <f ca="1">IF(G47&gt;=6,D43,E43)</f>
+        <v>1</v>
+      </c>
+      <c r="F56" s="20">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="G56" s="18"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="F57" s="20"/>
+      <c r="G57" s="18"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="47">
+        <f ca="1">D51*2^C51+D52*2^C52+D53*2^C53+D54*2^C54+D55*2^C55+D56*2^C56</f>
+        <v>32</v>
+      </c>
+      <c r="E58" s="47">
+        <f ca="1">E51*2^C51+E52*2^C52+E53*2^C53+E54*2^C54+E55*2^C55+E56*2^C56</f>
+        <v>19</v>
+      </c>
+      <c r="F58" s="20"/>
+      <c r="G58" s="18"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="54">
+        <f ca="1">FLOOR($B$32*H35,1)</f>
+        <v>2</v>
+      </c>
+      <c r="I60" s="54">
+        <f ca="1">FLOOR($B$32*I35,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C63" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C64" s="20">
+        <v>5</v>
+      </c>
+      <c r="D64" s="46">
+        <f ca="1">IF(H60=1,IF(D51=1,0,1),D51)</f>
+        <v>1</v>
+      </c>
+      <c r="E64" s="46">
+        <f ca="1">IF(I60=1,IF(E51=1,0,1),E51)</f>
+        <v>1</v>
+      </c>
+      <c r="F64" s="20">
+        <f>2^C64</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C65" s="20">
+        <v>4</v>
+      </c>
+      <c r="D65" s="46">
+        <f ca="1">IF(H60=2,IF(D52=1,0,1),D52)</f>
+        <v>1</v>
+      </c>
+      <c r="E65" s="46">
+        <f ca="1">IF(I60=2,IF(E52=1,0,1),E52)</f>
+        <v>1</v>
+      </c>
+      <c r="F65" s="20">
+        <f t="shared" ref="F65:F69" si="10">2^C65</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C66" s="20">
+        <v>3</v>
+      </c>
+      <c r="D66" s="46">
+        <f ca="1">IF(H60=3,IF(D53=1,0,1),D53)</f>
+        <v>0</v>
+      </c>
+      <c r="E66" s="46">
+        <f ca="1">IF(I60=3,IF(E53=1,0,1),E53)</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="20">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="20">
+        <v>2</v>
+      </c>
+      <c r="D67" s="46">
+        <f ca="1">IF(H60=4,IF(D54=1,0,1),D54)</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="46">
+        <f ca="1">IF(I60=4,IF(E54=1,0,1),E54)</f>
+        <v>0</v>
+      </c>
+      <c r="F67" s="20">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="20">
+        <v>1</v>
+      </c>
+      <c r="D68" s="46">
+        <f ca="1">IF(H60=5,IF(D55=1,0,1),D55)</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="46">
+        <f ca="1">IF(I60=5,IF(E55=1,0,1),E55)</f>
+        <v>1</v>
+      </c>
+      <c r="F68" s="20">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="20">
+        <v>0</v>
+      </c>
+      <c r="D69" s="46">
+        <f ca="1">IF(H60=6,IF(D56=1,0,1),D56)</f>
+        <v>0</v>
+      </c>
+      <c r="E69" s="46">
+        <f ca="1">IF(I60=6,IF(E56=1,0,1),E56)</f>
+        <v>1</v>
+      </c>
+      <c r="F69" s="20">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="20"/>
+      <c r="D70" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="E70" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="F70" s="20"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C71" s="20"/>
+      <c r="D71" s="47">
+        <f ca="1">D64*2^C64+D65*2^C65+D66*2^C66+D67*2^C67+D68*2^C68+D69*2^C69</f>
+        <v>48</v>
+      </c>
+      <c r="E71" s="47">
+        <f ca="1">E64*2^C64+E65*2^C65+E66*2^C66+E67*2^C67+E68*2^C68+E69*2^C69</f>
+        <v>51</v>
+      </c>
+      <c r="F71" s="20"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="55">
+        <f ca="1">(D71/C33)*(F35-C35)+C35</f>
+        <v>0.52380952380952372</v>
+      </c>
+      <c r="E73" s="55">
+        <f ca="1">(E71/C33)*(F35-C35)+F35</f>
+        <v>2.6190476190476191</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD98361-ECC4-4800-AA9F-4B889DA007F9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -9712,7 +12333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA823BB-9C8B-445A-82C8-B96D6661DC7D}">
   <dimension ref="A1:H101"/>
   <sheetViews>
@@ -9723,10 +12344,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="2"/>
       <c r="D1" t="s">
         <v>3</v>
@@ -9742,8 +12363,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="2" cm="1">
         <f t="array" ref="C2:C101">_xlfn.SEQUENCE(100,1,0,0.02)</f>
         <v>0</v>
@@ -9760,8 +12381,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="2">
         <v>0.02</v>
       </c>
@@ -9777,8 +12398,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="2">
         <v>0.04</v>
       </c>
@@ -9794,8 +12415,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="2">
         <v>0.06</v>
       </c>
@@ -9805,8 +12426,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="2">
         <v>0.08</v>
       </c>
@@ -9822,8 +12443,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="2">
         <v>0.1</v>
       </c>
@@ -9833,8 +12454,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="2">
         <v>0.12000000000000001</v>
       </c>
@@ -9844,8 +12465,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="2">
         <v>0.14000000000000001</v>
       </c>
@@ -9855,8 +12476,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="2">
         <v>0.16</v>
       </c>
@@ -9866,8 +12487,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="2">
         <v>0.18</v>
       </c>
@@ -9877,8 +12498,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="2">
         <v>0.19999999999999998</v>
       </c>
@@ -10694,4 +13315,19 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67700BCB-9B68-44F8-BC07-9ACE6C32C97C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected GA results scaling
</commit_message>
<xml_diff>
--- a/DSO.xlsx
+++ b/DSO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/kwl1y19_soton_ac_uk/Documents/UoS_2023_24/FEEG_DSO/Workbook/DSO-Workbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8217" documentId="8_{42FA694E-ED08-47C7-945B-F9D07721EF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81E4BE68-F375-4572-9083-5877CC1119AC}"/>
+  <xr:revisionPtr revIDLastSave="8218" documentId="8_{42FA694E-ED08-47C7-945B-F9D07721EF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB7F2B89-8DF0-4878-AAC1-3081B34E9FB0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{16D0D9C5-2E23-4080-8275-B376E5887C88}"/>
   </bookViews>
@@ -909,6 +909,29 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -934,29 +957,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5674,10 +5674,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="49"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -5695,8 +5695,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
       <c r="C5">
         <v>0</v>
       </c>
@@ -5712,8 +5712,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
       <c r="C6">
         <v>0.2</v>
       </c>
@@ -5729,8 +5729,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
       <c r="C7">
         <v>0.4</v>
       </c>
@@ -5746,8 +5746,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
       <c r="C8">
         <v>0.6</v>
       </c>
@@ -5757,8 +5757,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
       <c r="C9">
         <v>0.8</v>
       </c>
@@ -5774,8 +5774,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -5785,8 +5785,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
       <c r="C11">
         <v>1.2</v>
       </c>
@@ -5796,8 +5796,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
       <c r="C12">
         <v>1.4</v>
       </c>
@@ -5807,8 +5807,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
       <c r="C13">
         <v>1.6</v>
       </c>
@@ -5818,8 +5818,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
       <c r="C14">
         <v>1.8</v>
       </c>
@@ -5829,8 +5829,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
       <c r="C15">
         <v>2</v>
       </c>
@@ -6266,10 +6266,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S23" s="36" t="s">
+      <c r="S23" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="T23" s="36"/>
+      <c r="T23" s="51"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24">
@@ -6683,7 +6683,7 @@
       </c>
     </row>
     <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="47" t="s">
         <v>36</v>
       </c>
       <c r="B31">
@@ -6736,7 +6736,7 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
+      <c r="A32" s="50"/>
       <c r="B32">
         <v>2</v>
       </c>
@@ -6788,7 +6788,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+      <c r="A33" s="50"/>
       <c r="B33">
         <v>3</v>
       </c>
@@ -6840,7 +6840,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="50"/>
       <c r="B34">
         <v>4</v>
       </c>
@@ -6889,7 +6889,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="50"/>
       <c r="B35">
         <v>5</v>
       </c>
@@ -6938,7 +6938,7 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="50"/>
       <c r="B36">
         <v>6</v>
       </c>
@@ -6987,7 +6987,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+      <c r="A37" s="50"/>
       <c r="B37">
         <v>7</v>
       </c>
@@ -7036,7 +7036,7 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
+      <c r="A38" s="50"/>
       <c r="B38">
         <v>8</v>
       </c>
@@ -7085,7 +7085,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
+      <c r="A39" s="50"/>
       <c r="B39">
         <v>9</v>
       </c>
@@ -7134,7 +7134,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
+      <c r="A40" s="50"/>
       <c r="B40">
         <v>10</v>
       </c>
@@ -7233,7 +7233,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="47" t="s">
         <v>40</v>
       </c>
       <c r="B43">
@@ -7283,7 +7283,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
+      <c r="A44" s="50"/>
       <c r="B44">
         <v>2</v>
       </c>
@@ -7333,7 +7333,7 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="50"/>
       <c r="B45">
         <v>3</v>
       </c>
@@ -7383,7 +7383,7 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="50"/>
       <c r="B46">
         <v>4</v>
       </c>
@@ -7433,7 +7433,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
+      <c r="A47" s="50"/>
       <c r="B47">
         <v>5</v>
       </c>
@@ -7483,7 +7483,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
+      <c r="A48" s="50"/>
       <c r="B48">
         <v>6</v>
       </c>
@@ -7533,7 +7533,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+      <c r="A49" s="50"/>
       <c r="B49">
         <v>7</v>
       </c>
@@ -7583,7 +7583,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
+      <c r="A50" s="50"/>
       <c r="B50">
         <v>8</v>
       </c>
@@ -7633,7 +7633,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+      <c r="A51" s="50"/>
       <c r="B51">
         <v>9</v>
       </c>
@@ -7683,7 +7683,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="A52" s="50"/>
       <c r="B52">
         <v>10</v>
       </c>
@@ -7760,7 +7760,7 @@
       <c r="K54" s="17"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
+      <c r="A55" s="47" t="s">
         <v>44</v>
       </c>
       <c r="B55">
@@ -7789,7 +7789,7 @@
       <c r="K55" s="17"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="33"/>
+      <c r="A56" s="48"/>
       <c r="B56">
         <v>2</v>
       </c>
@@ -7821,7 +7821,7 @@
       <c r="K56" s="17"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
+      <c r="A57" s="48"/>
       <c r="B57">
         <v>3</v>
       </c>
@@ -7851,7 +7851,7 @@
       <c r="K57" s="17"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="33"/>
+      <c r="A58" s="48"/>
       <c r="B58">
         <v>4</v>
       </c>
@@ -7881,7 +7881,7 @@
       <c r="K58" s="17"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="33"/>
+      <c r="A59" s="48"/>
       <c r="B59">
         <v>5</v>
       </c>
@@ -7911,7 +7911,7 @@
       <c r="K59" s="17"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
+      <c r="A60" s="48"/>
       <c r="B60">
         <v>6</v>
       </c>
@@ -7937,7 +7937,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
+      <c r="A61" s="48"/>
       <c r="B61">
         <v>7</v>
       </c>
@@ -7963,7 +7963,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
+      <c r="A62" s="48"/>
       <c r="B62">
         <v>8</v>
       </c>
@@ -7989,7 +7989,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
+      <c r="A63" s="48"/>
       <c r="B63">
         <v>9</v>
       </c>
@@ -8015,7 +8015,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="33"/>
+      <c r="A64" s="48"/>
       <c r="B64">
         <v>10</v>
       </c>
@@ -8041,7 +8041,7 @@
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
+      <c r="A65" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8159,14 +8159,14 @@
       <c r="A8" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38" t="s">
+      <c r="C8" s="52"/>
+      <c r="D8" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="53"/>
       <c r="T8" s="17"/>
       <c r="U8" s="17"/>
     </row>
@@ -8230,7 +8230,7 @@
       <c r="U9" s="17"/>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="54" t="s">
         <v>76</v>
       </c>
       <c r="C10">
@@ -8282,7 +8282,7 @@
       <c r="U10" s="17"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
+      <c r="A11" s="55"/>
       <c r="C11">
         <v>0.5</v>
       </c>
@@ -8332,7 +8332,7 @@
       <c r="U11" s="17"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="55"/>
       <c r="C12" s="15">
         <v>0.5</v>
       </c>
@@ -8382,7 +8382,7 @@
       <c r="U12" s="17"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="55"/>
       <c r="C13" s="15">
         <v>0.5</v>
       </c>
@@ -8432,7 +8432,7 @@
       <c r="U13" s="17"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="55"/>
       <c r="C14" s="15">
         <v>0.5</v>
       </c>
@@ -8482,7 +8482,7 @@
       <c r="U14" s="17"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="55"/>
       <c r="C15" s="15">
         <v>0.5</v>
       </c>
@@ -8535,7 +8535,7 @@
       <c r="U15" s="17"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
+      <c r="A16" s="55"/>
       <c r="C16" s="15">
         <v>0.5</v>
       </c>
@@ -11046,8 +11046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05066E6-B41F-499D-9F3E-6508D758A95E}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11063,12 +11063,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="32" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="33" t="s">
         <v>79</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -11119,7 +11119,7 @@
       <c r="H4" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
     </row>
@@ -11189,7 +11189,7 @@
         <v>-0.30000000000000004</v>
       </c>
       <c r="F7" s="18">
-        <f t="shared" ref="F7:F26" si="1">E7-E6</f>
+        <f t="shared" ref="F7:F20" si="1">E7-E6</f>
         <v>-0.60000000000000009</v>
       </c>
       <c r="G7" s="18" t="str">
@@ -11490,7 +11490,7 @@
         <v>87</v>
       </c>
       <c r="C20" s="18">
-        <f t="shared" ref="C20:C26" si="4">C19-$H$5</f>
+        <f t="shared" ref="C20" si="4">C19-$H$5</f>
         <v>-0.70000000000000007</v>
       </c>
       <c r="D20" s="18">
@@ -11682,33 +11682,33 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="44"/>
+      <c r="I29" s="35"/>
     </row>
     <row r="30" spans="1:10" ht="330" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="43" t="s">
+      <c r="J30" s="34" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="J31" s="43"/>
+      <c r="J31" s="34"/>
     </row>
     <row r="32" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="36" t="s">
         <v>101</v>
       </c>
       <c r="B32" s="18">
         <v>6</v>
       </c>
-      <c r="J32" s="43"/>
+      <c r="J32" s="34"/>
     </row>
     <row r="33" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="36" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="18">
@@ -11718,7 +11718,7 @@
         <f>(2^B32)-1</f>
         <v>63</v>
       </c>
-      <c r="J33" s="43"/>
+      <c r="J33" s="34"/>
     </row>
     <row r="34" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -11745,22 +11745,22 @@
       <c r="H34" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I34" s="44" t="s">
+      <c r="I34" s="35" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8">
         <v>-1</v>
       </c>
-      <c r="D35" s="55">
+      <c r="D35" s="46">
         <v>-0.42857000000000001</v>
       </c>
-      <c r="E35" s="55">
+      <c r="E35" s="46">
         <v>4.7620000000000003E-2</v>
       </c>
       <c r="F35" s="8">
@@ -11768,19 +11768,19 @@
       </c>
       <c r="G35" s="8">
         <f ca="1">RAND()</f>
-        <v>0.96456720362692883</v>
+        <v>0.22708705692717934</v>
       </c>
       <c r="H35" s="8">
         <f t="shared" ref="H35:I35" ca="1" si="7">RAND()</f>
-        <v>0.40430807618073339</v>
+        <v>0.58912304719602726</v>
       </c>
       <c r="I35" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>0.29281474835444654</v>
+        <v>0.28573981540343885</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="36" t="s">
         <v>111</v>
       </c>
       <c r="D36">
@@ -11795,12 +11795,12 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
-      <c r="C37" s="51" t="s">
+      <c r="C37" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51" t="s">
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42" t="s">
         <v>105</v>
       </c>
     </row>
@@ -11809,18 +11809,18 @@
         <v>103</v>
       </c>
       <c r="B38" s="8"/>
-      <c r="C38" s="50">
+      <c r="C38" s="41">
         <v>5</v>
       </c>
-      <c r="D38" s="49">
+      <c r="D38" s="40">
         <f>FLOOR(D36/2^C38,1)</f>
         <v>0</v>
       </c>
-      <c r="E38" s="49">
+      <c r="E38" s="40">
         <f>FLOOR(E36/2^C38,1)</f>
         <v>1</v>
       </c>
-      <c r="F38" s="50">
+      <c r="F38" s="41">
         <f>2^C38</f>
         <v>32</v>
       </c>
@@ -11830,18 +11830,18 @@
         <v>106</v>
       </c>
       <c r="B39" s="8"/>
-      <c r="C39" s="50">
+      <c r="C39" s="41">
         <v>4</v>
       </c>
-      <c r="D39" s="49">
+      <c r="D39" s="40">
         <f>FLOOR((D36-D38*2^C38)/(2^C39),1)</f>
         <v>1</v>
       </c>
-      <c r="E39" s="49">
+      <c r="E39" s="40">
         <f>FLOOR((E36-E38*2^C38)/(2^C39),1)</f>
         <v>0</v>
       </c>
-      <c r="F39" s="50">
+      <c r="F39" s="41">
         <f t="shared" ref="F39:F43" si="8">2^C39</f>
         <v>16</v>
       </c>
@@ -11851,18 +11851,18 @@
         <v>107</v>
       </c>
       <c r="B40" s="8"/>
-      <c r="C40" s="50">
+      <c r="C40" s="41">
         <v>3</v>
       </c>
-      <c r="D40" s="49">
+      <c r="D40" s="40">
         <f>FLOOR((D36-D38*2^C38-D39*2^C39)/(2^C40),1)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="49">
+      <c r="E40" s="40">
         <f>FLOOR((E36-E38*2^C38-E39*2^C39)/(2^C40),1)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="50">
+      <c r="F40" s="41">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
@@ -11872,18 +11872,18 @@
         <v>108</v>
       </c>
       <c r="B41" s="8"/>
-      <c r="C41" s="50">
+      <c r="C41" s="41">
         <v>2</v>
       </c>
-      <c r="D41" s="49">
+      <c r="D41" s="40">
         <f>FLOOR((D36-D38*2^C38-D39*2^C39-D40*2^C40)/(2^C41),1)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="49">
+      <c r="E41" s="40">
         <f>FLOOR((E36-E38*2^C38-E39*2^C39-E40*2^C40)/(2^C41),1)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="50">
+      <c r="F41" s="41">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
@@ -11891,18 +11891,18 @@
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
-      <c r="C42" s="50">
+      <c r="C42" s="41">
         <v>1</v>
       </c>
-      <c r="D42" s="49">
+      <c r="D42" s="40">
         <f>FLOOR((D36-D38*2^C38-D39*2^C39-D40*2^C40-D41*2^C41)/(2^C42),1)</f>
         <v>1</v>
       </c>
-      <c r="E42" s="49">
+      <c r="E42" s="40">
         <f>FLOOR((E36-E38*2^C38-E39*2^C39-E40*2^C40-E41*2^C41)/(2^C42),1)</f>
         <v>0</v>
       </c>
-      <c r="F42" s="50">
+      <c r="F42" s="41">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
@@ -11910,18 +11910,18 @@
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
-      <c r="C43" s="50">
+      <c r="C43" s="41">
         <v>0</v>
       </c>
-      <c r="D43" s="49">
+      <c r="D43" s="40">
         <f>FLOOR((D36-D38*2^C38-D39*2^C39-D40*2^C40-D41*2^C41-D42*2^C42)/(2^C43),1)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="49">
+      <c r="E43" s="40">
         <f>FLOOR((E36-E38*2^C38-E39*2^C39-E40*2^C40-E41*2^C41-E42*2^C42)/(2^C43),1)</f>
         <v>1</v>
       </c>
-      <c r="F43" s="50">
+      <c r="F43" s="41">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
@@ -11929,30 +11929,30 @@
     <row r="44" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="51" t="s">
+      <c r="C44" s="41"/>
+      <c r="D44" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="E44" s="51" t="s">
+      <c r="E44" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="50"/>
+      <c r="F44" s="41"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>115</v>
       </c>
       <c r="B45" s="8"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="53">
+      <c r="C45" s="41"/>
+      <c r="D45" s="44">
         <f>D38*2^C38+D39*2^C39+D40*2^C40+D41*2^C41+D42*2^C42+D43*2^C43</f>
         <v>18</v>
       </c>
-      <c r="E45" s="53">
+      <c r="E45" s="44">
         <f>E38*2^C38+E39*2^C39+E40*2^C40+E41*2^C41+E42*2^C42+E43*2^C43</f>
         <v>33</v>
       </c>
-      <c r="F45" s="50"/>
+      <c r="F45" s="41"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
@@ -11963,9 +11963,9 @@
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="54">
+      <c r="G47" s="45">
         <f ca="1">FLOOR($B$32*G35,1)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -11978,12 +11978,12 @@
         <v>114</v>
       </c>
       <c r="B50" s="8"/>
-      <c r="C50" s="52" t="s">
+      <c r="C50" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52" t="s">
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43" t="s">
         <v>105</v>
       </c>
       <c r="G50" s="18"/>
@@ -11994,11 +11994,11 @@
       <c r="C51" s="20">
         <v>5</v>
       </c>
-      <c r="D51" s="46">
+      <c r="D51" s="37">
         <f ca="1">IF(G47&gt;=1,E38,D38)</f>
         <v>1</v>
       </c>
-      <c r="E51" s="46">
+      <c r="E51" s="37">
         <f ca="1">IF(G47&gt;=1,D38,E38)</f>
         <v>0</v>
       </c>
@@ -12014,13 +12014,13 @@
       <c r="C52" s="20">
         <v>4</v>
       </c>
-      <c r="D52" s="46">
+      <c r="D52" s="37">
         <f ca="1">IF(G47&gt;=2,E39,D39)</f>
+        <v>1</v>
+      </c>
+      <c r="E52" s="37">
+        <f ca="1">IF(G47&gt;=2,D39,E39)</f>
         <v>0</v>
-      </c>
-      <c r="E52" s="46">
-        <f ca="1">IF(G47&gt;=2,D39,E39)</f>
-        <v>1</v>
       </c>
       <c r="F52" s="20">
         <f t="shared" ref="F52:F56" si="9">2^C52</f>
@@ -12034,11 +12034,11 @@
       <c r="C53" s="20">
         <v>3</v>
       </c>
-      <c r="D53" s="46">
+      <c r="D53" s="37">
         <f ca="1">IF(G47&gt;=3,E40,D40)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="46">
+      <c r="E53" s="37">
         <f ca="1">IF(G47&gt;=3,D40,E40)</f>
         <v>0</v>
       </c>
@@ -12054,11 +12054,11 @@
       <c r="C54" s="20">
         <v>2</v>
       </c>
-      <c r="D54" s="46">
+      <c r="D54" s="37">
         <f ca="1">IF(G47&gt;=4,E41,D41)</f>
         <v>0</v>
       </c>
-      <c r="E54" s="46">
+      <c r="E54" s="37">
         <f ca="1">IF(G47&gt;=4,D41,E41)</f>
         <v>0</v>
       </c>
@@ -12074,13 +12074,13 @@
       <c r="C55" s="20">
         <v>1</v>
       </c>
-      <c r="D55" s="46">
+      <c r="D55" s="37">
         <f ca="1">IF(G47&gt;=5,E42,D42)</f>
+        <v>1</v>
+      </c>
+      <c r="E55" s="37">
+        <f ca="1">IF(G47&gt;=5,D42,E42)</f>
         <v>0</v>
-      </c>
-      <c r="E55" s="46">
-        <f ca="1">IF(G47&gt;=5,D42,E42)</f>
-        <v>1</v>
       </c>
       <c r="F55" s="20">
         <f t="shared" si="9"/>
@@ -12094,11 +12094,11 @@
       <c r="C56" s="20">
         <v>0</v>
       </c>
-      <c r="D56" s="46">
+      <c r="D56" s="37">
         <f ca="1">IF(G47&gt;=6,E43,D43)</f>
         <v>0</v>
       </c>
-      <c r="E56" s="46">
+      <c r="E56" s="37">
         <f ca="1">IF(G47&gt;=6,D43,E43)</f>
         <v>1</v>
       </c>
@@ -12112,10 +12112,10 @@
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="20"/>
-      <c r="D57" s="52" t="s">
+      <c r="D57" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="E57" s="52" t="s">
+      <c r="E57" s="43" t="s">
         <v>110</v>
       </c>
       <c r="F57" s="20"/>
@@ -12127,13 +12127,13 @@
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20"/>
-      <c r="D58" s="47">
+      <c r="D58" s="38">
         <f ca="1">D51*2^C51+D52*2^C52+D53*2^C53+D54*2^C54+D55*2^C55+D56*2^C56</f>
-        <v>32</v>
-      </c>
-      <c r="E58" s="47">
+        <v>50</v>
+      </c>
+      <c r="E58" s="38">
         <f ca="1">E51*2^C51+E52*2^C52+E53*2^C53+E54*2^C54+E55*2^C55+E56*2^C56</f>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F58" s="20"/>
       <c r="G58" s="18"/>
@@ -12155,22 +12155,22 @@
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
-      <c r="H60" s="54">
+      <c r="H60" s="45">
         <f ca="1">FLOOR($B$32*H35,1)</f>
-        <v>2</v>
-      </c>
-      <c r="I60" s="54">
+        <v>3</v>
+      </c>
+      <c r="I60" s="45">
         <f ca="1">FLOOR($B$32*I35,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="52" t="s">
+      <c r="C63" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52" t="s">
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43" t="s">
         <v>105</v>
       </c>
     </row>
@@ -12178,11 +12178,11 @@
       <c r="C64" s="20">
         <v>5</v>
       </c>
-      <c r="D64" s="46">
+      <c r="D64" s="37">
         <f ca="1">IF(H60=1,IF(D51=1,0,1),D51)</f>
         <v>1</v>
       </c>
-      <c r="E64" s="46">
+      <c r="E64" s="37">
         <f ca="1">IF(I60=1,IF(E51=1,0,1),E51)</f>
         <v>1</v>
       </c>
@@ -12195,13 +12195,13 @@
       <c r="C65" s="20">
         <v>4</v>
       </c>
-      <c r="D65" s="46">
+      <c r="D65" s="37">
         <f ca="1">IF(H60=2,IF(D52=1,0,1),D52)</f>
         <v>1</v>
       </c>
-      <c r="E65" s="46">
+      <c r="E65" s="37">
         <f ca="1">IF(I60=2,IF(E52=1,0,1),E52)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" s="20">
         <f t="shared" ref="F65:F69" si="10">2^C65</f>
@@ -12212,11 +12212,11 @@
       <c r="C66" s="20">
         <v>3</v>
       </c>
-      <c r="D66" s="46">
+      <c r="D66" s="37">
         <f ca="1">IF(H60=3,IF(D53=1,0,1),D53)</f>
-        <v>0</v>
-      </c>
-      <c r="E66" s="46">
+        <v>1</v>
+      </c>
+      <c r="E66" s="37">
         <f ca="1">IF(I60=3,IF(E53=1,0,1),E53)</f>
         <v>0</v>
       </c>
@@ -12229,11 +12229,11 @@
       <c r="C67" s="20">
         <v>2</v>
       </c>
-      <c r="D67" s="46">
+      <c r="D67" s="37">
         <f ca="1">IF(H60=4,IF(D54=1,0,1),D54)</f>
         <v>0</v>
       </c>
-      <c r="E67" s="46">
+      <c r="E67" s="37">
         <f ca="1">IF(I60=4,IF(E54=1,0,1),E54)</f>
         <v>0</v>
       </c>
@@ -12246,13 +12246,13 @@
       <c r="C68" s="20">
         <v>1</v>
       </c>
-      <c r="D68" s="46">
+      <c r="D68" s="37">
         <f ca="1">IF(H60=5,IF(D55=1,0,1),D55)</f>
+        <v>1</v>
+      </c>
+      <c r="E68" s="37">
+        <f ca="1">IF(I60=5,IF(E55=1,0,1),E55)</f>
         <v>0</v>
-      </c>
-      <c r="E68" s="46">
-        <f ca="1">IF(I60=5,IF(E55=1,0,1),E55)</f>
-        <v>1</v>
       </c>
       <c r="F68" s="20">
         <f t="shared" si="10"/>
@@ -12263,11 +12263,11 @@
       <c r="C69" s="20">
         <v>0</v>
       </c>
-      <c r="D69" s="46">
+      <c r="D69" s="37">
         <f ca="1">IF(H60=6,IF(D56=1,0,1),D56)</f>
         <v>0</v>
       </c>
-      <c r="E69" s="46">
+      <c r="E69" s="37">
         <f ca="1">IF(I60=6,IF(E56=1,0,1),E56)</f>
         <v>1</v>
       </c>
@@ -12278,23 +12278,23 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C70" s="20"/>
-      <c r="D70" s="52" t="s">
+      <c r="D70" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="E70" s="52" t="s">
+      <c r="E70" s="43" t="s">
         <v>110</v>
       </c>
       <c r="F70" s="20"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C71" s="20"/>
-      <c r="D71" s="47">
+      <c r="D71" s="38">
         <f ca="1">D64*2^C64+D65*2^C65+D66*2^C66+D67*2^C67+D68*2^C68+D69*2^C69</f>
-        <v>48</v>
-      </c>
-      <c r="E71" s="47">
+        <v>58</v>
+      </c>
+      <c r="E71" s="38">
         <f ca="1">E64*2^C64+E65*2^C65+E66*2^C66+E67*2^C67+E68*2^C68+E69*2^C69</f>
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F71" s="20"/>
     </row>
@@ -12304,13 +12304,13 @@
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
-      <c r="D73" s="55">
+      <c r="D73" s="46">
         <f ca="1">(D71/C33)*(F35-C35)+C35</f>
-        <v>0.52380952380952372</v>
-      </c>
-      <c r="E73" s="55">
-        <f ca="1">(E71/C33)*(F35-C35)+F35</f>
-        <v>2.6190476190476191</v>
+        <v>0.84126984126984117</v>
+      </c>
+      <c r="E73" s="46">
+        <f ca="1">(E71/C33)*(F35-C35)+C35</f>
+        <v>4.7619047619047672E-2</v>
       </c>
     </row>
   </sheetData>
@@ -12344,10 +12344,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="49"/>
       <c r="C1" s="2"/>
       <c r="D1" t="s">
         <v>3</v>
@@ -12363,8 +12363,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
       <c r="C2" s="2" cm="1">
         <f t="array" ref="C2:C101">_xlfn.SEQUENCE(100,1,0,0.02)</f>
         <v>0</v>
@@ -12381,8 +12381,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="2">
         <v>0.02</v>
       </c>
@@ -12398,8 +12398,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="2">
         <v>0.04</v>
       </c>
@@ -12415,8 +12415,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="2">
         <v>0.06</v>
       </c>
@@ -12426,8 +12426,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="2">
         <v>0.08</v>
       </c>
@@ -12443,8 +12443,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="2">
         <v>0.1</v>
       </c>
@@ -12454,8 +12454,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="2">
         <v>0.12000000000000001</v>
       </c>
@@ -12465,8 +12465,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="2">
         <v>0.14000000000000001</v>
       </c>
@@ -12476,8 +12476,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="2">
         <v>0.16</v>
       </c>
@@ -12487,8 +12487,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="2">
         <v>0.18</v>
       </c>
@@ -12498,8 +12498,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="2">
         <v>0.19999999999999998</v>
       </c>

</xml_diff>